<commit_message>
Added Standard Deviation Tables
</commit_message>
<xml_diff>
--- a/SortingProject/Sorting Report Project.xlsx
+++ b/SortingProject/Sorting Report Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\College\115\SortingProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA042229-CCDC-46A1-B110-A95C276B52C9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25ECB9F-9DB8-425E-A0A1-E80D912E6D5D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" tabRatio="596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="28">
   <si>
     <t>Random</t>
   </si>
@@ -97,15 +97,33 @@
   <si>
     <t>Quick Sort Total Average Running Time</t>
   </si>
+  <si>
+    <t>std dev.</t>
+  </si>
+  <si>
+    <t>Bubble Sort Standard Deviation</t>
+  </si>
+  <si>
+    <t>Insertion Sort Standard Deviation</t>
+  </si>
+  <si>
+    <t>Merge Sort Standard Deviation</t>
+  </si>
+  <si>
+    <t>Quick Sort Standard Deviation</t>
+  </si>
+  <si>
+    <t>Selection Sort Standard Deviation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="0.000000000"/>
-    <numFmt numFmtId="166" formatCode="0.000000000\ &quot;s&quot;"/>
-    <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000\ &quot;s&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -358,41 +376,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -402,8 +408,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -414,6 +429,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -480,46 +504,70 @@
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="52">
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="165" formatCode="0.000000000\ &quot;s&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="165" formatCode="0.000000000\ &quot;s&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="165" formatCode="0.000000000\ &quot;s&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="165" formatCode="0.000000000\ &quot;s&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right/>
         <top/>
         <bottom/>
@@ -535,7 +583,74 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -548,13 +663,13 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -569,25 +684,42 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000\ &quot;s&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.000000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="165" formatCode="0.000000000\ &quot;s&quot;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.000000000\ &quot;s&quot;"/>
+      <numFmt numFmtId="165" formatCode="0.000000000\ &quot;s&quot;"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1090,57 +1222,63 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Master!$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>Master!$A$21:$A$26</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+            <c:numRef>
+              <c:f>Master!$A$22:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Size</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>1000000</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Master!$B$21:$B$26</c:f>
+              <c:f>Master!$B$22:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>0.000000\ "s"</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.2133000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2133000000000001E-5</c:v>
+                  <c:v>0.10868792499999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.10868792499999999</c:v>
+                  <c:v>10.474407243000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.474407243000002</c:v>
+                  <c:v>72.722735130000018</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>72.722735130000018</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>300.00122177666663</c:v>
                 </c:pt>
               </c:numCache>
@@ -1156,57 +1294,63 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Master!$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ordered</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>Master!$A$21:$A$26</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+            <c:numRef>
+              <c:f>Master!$A$22:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Size</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>1000000</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Master!$C$21:$C$26</c:f>
+              <c:f>Master!$C$22:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>0.000000\ "s"</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.164E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.164E-6</c:v>
+                  <c:v>4.2731500000000005E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.2731500000000005E-4</c:v>
+                  <c:v>4.1180310000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.1180310000000003E-3</c:v>
+                  <c:v>2.2213900000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2213900000000002E-4</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>0.39652009399999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -1222,57 +1366,63 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Master!$D$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Reverse</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>Master!$A$21:$A$26</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+            <c:numRef>
+              <c:f>Master!$A$22:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Size</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>1000000</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Master!$D$21:$D$26</c:f>
+              <c:f>Master!$D$22:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>0.000000\ "s"</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.3995000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3995000000000003E-5</c:v>
+                  <c:v>0.216164258</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.216164258</c:v>
+                  <c:v>21.165291976999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.165291976999999</c:v>
+                  <c:v>136.800524981</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>136.800524981</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>300.00114007333337</c:v>
                 </c:pt>
               </c:numCache>
@@ -1288,57 +1438,63 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Master!$E$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Shuffled</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>Master!$A$21:$A$26</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+            <c:numRef>
+              <c:f>Master!$A$22:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Size</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>1000000</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Master!$E$21:$E$26</c:f>
+              <c:f>Master!$E$22:$E$26</c:f>
               <c:numCache>
                 <c:formatCode>0.000000\ "s"</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8.9109999999999999E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.9109999999999999E-6</c:v>
+                  <c:v>3.5311202999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5311202999999999E-2</c:v>
+                  <c:v>3.1876187959999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.1876187959999998</c:v>
+                  <c:v>4.9872695050000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9872695050000004</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>300.00124903833336</c:v>
                 </c:pt>
               </c:numCache>
@@ -2889,28 +3045,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B03BC507-47CA-4FB4-BA8B-812C723A72D6}" name="Table1" displayName="Table1" ref="A2:E7" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B03BC507-47CA-4FB4-BA8B-812C723A72D6}" name="Table1" displayName="Table1" ref="A2:E7" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="A2:E7" xr:uid="{55F75185-D20C-48C8-B696-BF724D2EE809}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2B59EBED-F148-472E-B3CC-35F56499FBFA}" name="Size" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{611AA8CD-CA4E-42E6-B24F-1FAF5FFDD716}" name="Random" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{D8E66C9D-31A7-4A5A-8450-4442ABB0CB22}" name="Ordered" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{0B971BBB-0860-481B-A27E-9D2CA1761C69}" name="Reverse" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{B37CD649-980D-4E5F-BB26-023B7F7AFA86}" name="Shuffled" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{2B59EBED-F148-472E-B3CC-35F56499FBFA}" name="Size" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{611AA8CD-CA4E-42E6-B24F-1FAF5FFDD716}" name="Random" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{D8E66C9D-31A7-4A5A-8450-4442ABB0CB22}" name="Ordered" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{0B971BBB-0860-481B-A27E-9D2CA1761C69}" name="Reverse" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{B37CD649-980D-4E5F-BB26-023B7F7AFA86}" name="Shuffled" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{CFC8C86D-2879-4026-9B78-9AD3100AA927}" name="Table611" displayName="Table611" ref="A89:E94" totalsRowShown="0">
+  <autoFilter ref="A89:E94" xr:uid="{60978F90-BCF9-4E95-A05B-E73B1A585050}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{5F9A3A23-A1AC-4714-B850-B7BA65A1358B}" name="Size"/>
+    <tableColumn id="2" xr3:uid="{71F41CA0-C2C3-40AE-B046-7D37F6A0EA03}" name="Random" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{A25C535C-5E8A-4158-8A6D-1C6B360F984D}" name="Ordered" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{C253668C-284D-4843-B6C7-89410D8A12FD}" name="Reverse" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{7A3DDBED-3867-4D09-915B-3B83A95D5A01}" name="Shuffled" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2BA97E30-712D-463E-89FC-51AEF9144B57}" name="Table5" displayName="Table5" ref="A21:E26" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{2BA97E30-712D-463E-89FC-51AEF9144B57}" name="Table5" displayName="Table5" ref="A21:E26" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43">
   <autoFilter ref="A21:E26" xr:uid="{8384A188-D966-4ED1-8654-1B79630E1576}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1A7425BA-C2D8-472D-ABCC-19D422EDE935}" name="Size" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{B7903F84-77EE-4392-9738-47AE36B4C678}" name="Random" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{1F332253-44B9-4643-9492-A2F0AEED3302}" name="Ordered" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{9D4CD237-7415-487E-9403-3410395B67A8}" name="Reverse" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{98D7E314-19A6-41B7-8F9C-5B1F799DFE07}" name="Shuffled" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{1A7425BA-C2D8-472D-ABCC-19D422EDE935}" name="Size" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{B7903F84-77EE-4392-9738-47AE36B4C678}" name="Random" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{1F332253-44B9-4643-9492-A2F0AEED3302}" name="Ordered" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{9D4CD237-7415-487E-9403-3410395B67A8}" name="Reverse" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{98D7E314-19A6-41B7-8F9C-5B1F799DFE07}" name="Shuffled" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2921,10 +3091,10 @@
   <autoFilter ref="A81:E86" xr:uid="{1694555E-768A-425F-A68B-3D3556B79481}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{FF8584C4-45B5-4369-98C6-F4D61A1B7FC8}" name="Size"/>
-    <tableColumn id="2" xr3:uid="{88B7703B-F03E-474C-93FD-A63D844EDE3C}" name="Random" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{0C119381-E851-4677-911E-F2248B199993}" name="Ordered" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{3DC0CD6B-6141-4C84-9BAC-7391E94FA8CF}" name="Reverse" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{0F155D16-9C4F-474F-B5DE-682DF0F6FB5F}" name="Shuffled" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{88B7703B-F03E-474C-93FD-A63D844EDE3C}" name="Random" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{0C119381-E851-4677-911E-F2248B199993}" name="Ordered" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{3DC0CD6B-6141-4C84-9BAC-7391E94FA8CF}" name="Reverse" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{0F155D16-9C4F-474F-B5DE-682DF0F6FB5F}" name="Shuffled" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2935,10 +3105,10 @@
   <autoFilter ref="A41:E46" xr:uid="{BB82E160-F3BC-43D2-A376-88EED58224C0}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D2010592-7F6D-4292-84A2-04AC526CC7DE}" name="Size"/>
-    <tableColumn id="2" xr3:uid="{A44F0D0F-D5C1-4033-833F-6691E551FE71}" name="Random" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{246C69AE-4F43-45AC-BEEA-AA9793FCC3FD}" name="Ordered" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{D92B61DD-5217-436A-A146-287A092A856E}" name="Reverse" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{1AC4AA7D-B33D-4819-8B9C-8FFB68AAC31A}" name="Shuffled" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{A44F0D0F-D5C1-4033-833F-6691E551FE71}" name="Random" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{246C69AE-4F43-45AC-BEEA-AA9793FCC3FD}" name="Ordered" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{D92B61DD-5217-436A-A146-287A092A856E}" name="Reverse" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{1AC4AA7D-B33D-4819-8B9C-8FFB68AAC31A}" name="Shuffled" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2949,10 +3119,66 @@
   <autoFilter ref="A61:E66" xr:uid="{F980AD14-F6C3-4155-96ED-929C1DD894D6}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{5517D46F-BD2B-47BA-9289-526AFDD7EE02}" name="Size"/>
-    <tableColumn id="2" xr3:uid="{EA3EFA3D-58DA-4E4E-975B-1F58B597EBCD}" name="Random" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{5E37328A-14A6-450C-BE40-0921D1FA116E}" name="Ordered" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{FE20EE39-1DC7-4D0F-A8C1-9A88F8F16968}" name="Reverse" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{9FFFD5C8-C885-4783-AFE1-3397423C29DC}" name="Shuffled" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{EA3EFA3D-58DA-4E4E-975B-1F58B597EBCD}" name="Random" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{5E37328A-14A6-450C-BE40-0921D1FA116E}" name="Ordered" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{FE20EE39-1DC7-4D0F-A8C1-9A88F8F16968}" name="Reverse" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{9FFFD5C8-C885-4783-AFE1-3397423C29DC}" name="Shuffled" dataDxfId="26"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E029CA2B-A502-4B0B-9A5C-6B3884181DE3}" name="Table13" displayName="Table13" ref="A10:E15" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A10:E15" xr:uid="{AE3FEABB-3932-457F-99AD-67ADBDC2A814}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{5213B2DA-55FF-4A0F-9A99-167D9EA64086}" name="Size" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{568F4C8F-B838-437C-94DE-7624E8F5D2B8}" name="Random" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{344A49C3-E678-4D11-8EFC-DDA502AA8D0E}" name="Ordered" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{429F7965-74E4-4B8F-8023-95F4219CFF9F}" name="Reverse" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{975F8F37-19D3-44B8-8F23-F24ACF07C6A4}" name="Shuffled" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E1549576-56D8-4B34-B4BA-283B592CD072}" name="Table54" displayName="Table54" ref="A29:E34" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17">
+  <autoFilter ref="A29:E34" xr:uid="{936E8F8A-741E-445A-8B32-E1525B256A40}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{4CF722D3-8371-4FC9-A695-C92B944B6848}" name="Size" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{17748E1A-7C10-46F1-80A2-B4BBFEA006F4}" name="Random" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{4B8C7698-CAB3-4E4B-B23F-DE91E7B3D938}" name="Ordered" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{E99F8AD5-7A1F-417E-BF77-FE3FD5174BAD}" name="Reverse" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{238EBA99-0F63-44FB-9D76-E6554C084445}" name="Shuffled" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{436ABE4F-13A4-4F68-BDCF-DD40E337B852}" name="Table75" displayName="Table75" ref="A50:E55" totalsRowShown="0">
+  <autoFilter ref="A50:E55" xr:uid="{7C21D96D-3E89-4AA7-B29F-1A7A44C7AD34}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{D3C5ACD4-AEBD-4FE3-8F4F-20EE4BF851DC}" name="Size"/>
+    <tableColumn id="2" xr3:uid="{85978DBF-6317-4C9B-9F6C-FB22ABFFF40A}" name="Random" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{49BD77D5-F13D-4A00-8440-433B562F17C2}" name="Ordered" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{6E376C91-EE9A-4140-B10D-34B10224EBE9}" name="Reverse" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{10191F29-8B5A-40AB-9B22-FBFCA33ECDA9}" name="Shuffled" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{401A51A2-C6F4-45C6-B7ED-47F6A32EC92B}" name="Table810" displayName="Table810" ref="A69:E74" totalsRowShown="0">
+  <autoFilter ref="A69:E74" xr:uid="{4ED6BC5C-A74C-489E-A6D5-9EF1D1D47AD2}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{01DD000F-CF15-4E1A-8EA2-B7C39766CBC4}" name="Size"/>
+    <tableColumn id="2" xr3:uid="{39C3437D-F1CA-4355-827A-094440C6E22A}" name="Random" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{BA0A958F-4576-422C-B965-3711FEA3F550}" name="Ordered" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{AF945967-0C1C-4EFC-BDE5-B1993D536D07}" name="Reverse" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{90BA2A95-219C-405D-A961-74208BF9BEEF}" name="Shuffled" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3282,8 +3508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="A20:E26"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="F85" sqref="F85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3295,275 +3521,497 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>10</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <f>'Bubble Sort'!E103</f>
         <v>3.7633999999999992E-5</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <f>'Bubble Sort'!F103</f>
         <v>4.8539999999999996E-6</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <f>'Bubble Sort'!G103</f>
         <v>4.4233545454545451E-5</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <f>'Bubble Sort'!H103</f>
         <v>2.5296E-5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>1000</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <f>'Bubble Sort'!N103</f>
         <v>0.38218852199999997</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <f>'Bubble Sort'!O103</f>
         <v>4.2489999999999992E-4</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <f>'Bubble Sort'!P103</f>
         <v>0.41176638300000007</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <f>'Bubble Sort'!Q103</f>
         <v>0.38505956299999999</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>10000</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <f>'Bubble Sort'!W103</f>
         <v>40.460980575000001</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <f>'Bubble Sort'!X103</f>
         <v>4.099890000000001E-3</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <f>'Bubble Sort'!Y103</f>
         <v>46.768684055999998</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <f>'Bubble Sort'!Z103</f>
         <v>43.140773276999994</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>100000</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <f>'Bubble Sort'!AF103</f>
         <v>105.19817065800001</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <f>'Bubble Sort'!AG103</f>
         <v>3.0981800000000001E-4</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <f>'Bubble Sort'!AH103</f>
         <v>143.15112576000001</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <f>'Bubble Sort'!AI103</f>
         <v>12.099274613000002</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>1000000</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <f>'Bubble Sort'!AO103</f>
         <v>300.00120614666668</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <f>'Bubble Sort'!AP103</f>
         <v>0.39579532299999992</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <f>'Bubble Sort'!AQ103</f>
         <v>300.00126811666661</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <f>'Bubble Sort'!AR103</f>
         <v>300.00177902000001</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7">
+        <v>1.470327387442207E-6</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1.4070113034658974E-6</v>
+      </c>
+      <c r="D11" s="7">
+        <v>5.5527839045751681E-6</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1.4750394618929408E-6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B12" s="7">
+        <v>2.5411264328230325E-3</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1.8800075220137508E-5</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1.6969268538996765E-3</v>
+      </c>
+      <c r="E12" s="7">
+        <v>1.9606463604223395E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>10000</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0.86529379593060129</v>
+      </c>
+      <c r="C13" s="7">
+        <v>1.0555058866570462E-4</v>
+      </c>
+      <c r="D13" s="7">
+        <v>6.3345215171960865</v>
+      </c>
+      <c r="E13" s="7">
+        <v>6.2093088639306222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>100000</v>
+      </c>
+      <c r="B14" s="7">
+        <v>5.2580112643492445</v>
+      </c>
+      <c r="C14" s="7">
+        <v>3.8448302900903133E-5</v>
+      </c>
+      <c r="D14" s="7">
+        <v>11.508834093058141</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.12167377308712887</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="B15" s="7">
+        <v>1.9492205014851657E-4</v>
+      </c>
+      <c r="C15" s="7">
+        <v>9.4867000775141841E-4</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1.8428451650695369E-4</v>
+      </c>
+      <c r="E15" s="7">
+        <v>3.5724276574394267E-3</v>
+      </c>
+    </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="26"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="13">
+      <c r="A22" s="9">
         <v>10</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="10">
         <f>'Insertion Sort'!E103</f>
         <v>1.2133000000000001E-5</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="10">
         <f>'Insertion Sort'!F103</f>
         <v>5.164E-6</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="10">
         <f>'Insertion Sort'!G103</f>
         <v>2.3995000000000003E-5</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="11">
         <f>'Insertion Sort'!H103</f>
         <v>8.9109999999999999E-6</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="16">
+      <c r="A23" s="12">
         <v>1000</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="13">
         <f>'Insertion Sort'!N103</f>
         <v>0.10868792499999999</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="13">
         <f>'Insertion Sort'!O103</f>
         <v>4.2731500000000005E-4</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="13">
         <f>'Insertion Sort'!P103</f>
         <v>0.216164258</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E23" s="14">
         <f>'Insertion Sort'!Q103</f>
         <v>3.5311202999999999E-2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="16">
+      <c r="A24" s="12">
         <v>10000</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="13">
         <f>'Insertion Sort'!W103</f>
         <v>10.474407243000002</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="13">
         <f>'Insertion Sort'!X103</f>
         <v>4.1180310000000003E-3</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="13">
         <f>'Insertion Sort'!Y103</f>
         <v>21.165291976999999</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E24" s="14">
         <f>'Insertion Sort'!Z103</f>
         <v>3.1876187959999998</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="16">
+      <c r="A25" s="12">
         <v>100000</v>
       </c>
-      <c r="B25" s="17">
+      <c r="B25" s="13">
         <f>'Insertion Sort'!AF103</f>
         <v>72.722735130000018</v>
       </c>
-      <c r="C25" s="17">
+      <c r="C25" s="13">
         <f>'Insertion Sort'!AG103</f>
         <v>2.2213900000000002E-4</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="13">
         <f>'Insertion Sort'!AH103</f>
         <v>136.800524981</v>
       </c>
-      <c r="E25" s="18">
+      <c r="E25" s="14">
         <f>'Insertion Sort'!AI103</f>
         <v>4.9872695050000004</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="19">
+      <c r="A26" s="15">
         <v>1000000</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="16">
         <f>'Insertion Sort'!AO103</f>
         <v>300.00122177666663</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C26" s="16">
         <f>'Insertion Sort'!AP103</f>
         <v>0.39652009399999999</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="16">
         <f>'Insertion Sort'!AQ103</f>
         <v>300.00114007333337</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="17">
         <f>'Insertion Sort'!AR103</f>
         <v>300.00124903833336</v>
       </c>
     </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="29"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>10</v>
+      </c>
+      <c r="B30" s="31">
+        <v>1.7118422942561176E-7</v>
+      </c>
+      <c r="C30" s="31">
+        <v>9.9478640923567117E-7</v>
+      </c>
+      <c r="D30" s="31">
+        <v>2.2879736083100335E-6</v>
+      </c>
+      <c r="E30" s="32">
+        <v>1.7401671811012304E-7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="12">
+        <v>1000</v>
+      </c>
+      <c r="B31" s="33">
+        <v>9.963815235540048E-4</v>
+      </c>
+      <c r="C31" s="33">
+        <v>1.5392411714342832E-5</v>
+      </c>
+      <c r="D31" s="33">
+        <v>5.8288469775689888E-3</v>
+      </c>
+      <c r="E31" s="34">
+        <v>3.9522798981132747E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="12">
+        <v>10000</v>
+      </c>
+      <c r="B32" s="33">
+        <v>1.8254461088417107E-2</v>
+      </c>
+      <c r="C32" s="33">
+        <v>1.2761044786000205E-4</v>
+      </c>
+      <c r="D32" s="33">
+        <v>0.47025357698834208</v>
+      </c>
+      <c r="E32" s="34">
+        <v>7.7188260918710531E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="12">
+        <v>100000</v>
+      </c>
+      <c r="B33" s="33">
+        <v>5.530829561711295</v>
+      </c>
+      <c r="C33" s="33">
+        <v>7.1561162651259333E-7</v>
+      </c>
+      <c r="D33" s="33">
+        <v>2.3010540984013677</v>
+      </c>
+      <c r="E33" s="34">
+        <v>0.20056533128894721</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="15">
+        <v>1000000</v>
+      </c>
+      <c r="B34" s="35">
+        <v>2.1708322383141515E-4</v>
+      </c>
+      <c r="C34" s="35">
+        <v>1.6913334252350045E-3</v>
+      </c>
+      <c r="D34" s="35">
+        <v>2.296116753316763E-4</v>
+      </c>
+      <c r="E34" s="36">
+        <v>2.5071576402001185E-4</v>
+      </c>
+    </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="28" t="s">
+      <c r="A40" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="30"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="29"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -3586,19 +4034,19 @@
       <c r="A42">
         <v>10</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42" s="7">
         <f>'Merge Sort'!E103</f>
         <v>3.8369999999999999E-6</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C42" s="7">
         <f>'Merge Sort'!F103</f>
         <v>3.3869999999999999E-6</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D42" s="7">
         <f>'Merge Sort'!G103</f>
         <v>3.4719999999999991E-6</v>
       </c>
-      <c r="E42" s="8">
+      <c r="E42" s="7">
         <f>'Merge Sort'!H103</f>
         <v>3.7790000000000002E-6</v>
       </c>
@@ -3607,19 +4055,19 @@
       <c r="A43">
         <v>1000</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" s="7">
         <f>'Merge Sort'!N103</f>
         <v>4.5182200000000005E-4</v>
       </c>
-      <c r="C43" s="8">
+      <c r="C43" s="7">
         <f>'Merge Sort'!O103</f>
         <v>3.9187900000000003E-4</v>
       </c>
-      <c r="D43" s="8">
+      <c r="D43" s="7">
         <f>'Merge Sort'!P103</f>
         <v>3.8273400000000003E-4</v>
       </c>
-      <c r="E43" s="8">
+      <c r="E43" s="7">
         <f>'Merge Sort'!Q103</f>
         <v>3.8561199999999997E-4</v>
       </c>
@@ -3628,19 +4076,19 @@
       <c r="A44">
         <v>10000</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44" s="7">
         <f>'Merge Sort'!W103</f>
         <v>3.52666E-3</v>
       </c>
-      <c r="C44" s="8">
+      <c r="C44" s="7">
         <f>'Merge Sort'!X103</f>
         <v>2.9998329999999995E-3</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D44" s="7">
         <f>'Merge Sort'!Y103</f>
         <v>2.8897610000000002E-3</v>
       </c>
-      <c r="E44" s="8">
+      <c r="E44" s="7">
         <f>'Merge Sort'!Z103</f>
         <v>3.0631809999999999E-3</v>
       </c>
@@ -3649,19 +4097,19 @@
       <c r="A45">
         <v>100000</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" s="7">
         <f>'Merge Sort'!AF103</f>
         <v>4.7896345999999992E-2</v>
       </c>
-      <c r="C45" s="8">
+      <c r="C45" s="7">
         <f>'Merge Sort'!AG103</f>
         <v>4.069722500000001E-2</v>
       </c>
-      <c r="D45" s="8">
+      <c r="D45" s="7">
         <f>'Merge Sort'!AH103</f>
         <v>4.0462286E-2</v>
       </c>
-      <c r="E45" s="8">
+      <c r="E45" s="7">
         <f>'Merge Sort'!AI103</f>
         <v>4.1825701999999999E-2</v>
       </c>
@@ -3670,31 +4118,142 @@
       <c r="A46">
         <v>1000000</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46" s="7">
         <f>'Merge Sort'!AO103</f>
         <v>0.49782594199999997</v>
       </c>
-      <c r="C46" s="8">
+      <c r="C46" s="7">
         <f>'Merge Sort'!AP103</f>
         <v>0.42080879800000009</v>
       </c>
-      <c r="D46" s="8">
+      <c r="D46" s="7">
         <f>'Merge Sort'!AQ103</f>
         <v>0.42141007600000002</v>
       </c>
-      <c r="E46" s="8">
+      <c r="E46" s="7">
         <f>'Merge Sort'!AR103</f>
         <v>0.42739784199999997</v>
       </c>
     </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="28"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="29"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>10</v>
+      </c>
+      <c r="B51" s="7">
+        <v>1.6695523503337799E-6</v>
+      </c>
+      <c r="C51" s="7">
+        <v>8.0524229367014222E-7</v>
+      </c>
+      <c r="D51" s="7">
+        <v>1.1447799841546905E-6</v>
+      </c>
+      <c r="E51" s="7">
+        <v>1.744792830166957E-6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1000</v>
+      </c>
+      <c r="B52" s="7">
+        <v>5.6920054835042489E-5</v>
+      </c>
+      <c r="C52" s="7">
+        <v>5.4301631009602555E-5</v>
+      </c>
+      <c r="D52" s="7">
+        <v>5.0802322821308116E-5</v>
+      </c>
+      <c r="E52" s="7">
+        <v>4.9964036116495887E-5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>10000</v>
+      </c>
+      <c r="B53" s="7">
+        <v>1.7525698245430881E-4</v>
+      </c>
+      <c r="C53" s="7">
+        <v>2.5038249005120627E-4</v>
+      </c>
+      <c r="D53" s="7">
+        <v>1.3628676310254673E-4</v>
+      </c>
+      <c r="E53" s="7">
+        <v>2.1338285016951253E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>100000</v>
+      </c>
+      <c r="B54" s="7">
+        <v>1.4084242268979647E-3</v>
+      </c>
+      <c r="C54" s="7">
+        <v>3.3661465676120559E-4</v>
+      </c>
+      <c r="D54" s="7">
+        <v>2.3527113952830973E-4</v>
+      </c>
+      <c r="E54" s="7">
+        <v>2.6734594316969322E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1000000</v>
+      </c>
+      <c r="B55" s="7">
+        <v>4.6078095028255737E-3</v>
+      </c>
+      <c r="C55" s="7">
+        <v>1.6366821042893495E-3</v>
+      </c>
+      <c r="D55" s="7">
+        <v>1.7182035205423236E-3</v>
+      </c>
+      <c r="E55" s="7">
+        <v>1.9109431687990618E-3</v>
+      </c>
+    </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="28" t="s">
+      <c r="A60" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B60" s="29"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="30"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="29"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
@@ -3717,19 +4276,19 @@
       <c r="A62">
         <v>10</v>
       </c>
-      <c r="B62" s="8">
+      <c r="B62" s="7">
         <f>'Quick Sort'!E103</f>
         <v>1.7680000000000001E-6</v>
       </c>
-      <c r="C62" s="8">
+      <c r="C62" s="7">
         <f>'Quick Sort'!F103</f>
         <v>1.579E-6</v>
       </c>
-      <c r="D62" s="8">
+      <c r="D62" s="7">
         <f>'Quick Sort'!G103</f>
         <v>1.7649999999999998E-6</v>
       </c>
-      <c r="E62" s="8">
+      <c r="E62" s="7">
         <f>'Quick Sort'!H103</f>
         <v>1.668E-6</v>
       </c>
@@ -3738,19 +4297,19 @@
       <c r="A63">
         <v>1000</v>
       </c>
-      <c r="B63" s="8">
+      <c r="B63" s="7">
         <f>'Quick Sort'!N103</f>
         <v>1.7525300000000002E-4</v>
       </c>
-      <c r="C63" s="8">
+      <c r="C63" s="7">
         <f>'Quick Sort'!O103</f>
         <v>8.0354999999999985E-5</v>
       </c>
-      <c r="D63" s="8">
+      <c r="D63" s="7">
         <f>'Quick Sort'!P103</f>
         <v>8.9680000000000009E-5</v>
       </c>
-      <c r="E63" s="8">
+      <c r="E63" s="7">
         <f>'Quick Sort'!Q103</f>
         <v>8.7863000000000009E-5</v>
       </c>
@@ -3759,19 +4318,19 @@
       <c r="A64">
         <v>10000</v>
       </c>
-      <c r="B64" s="8">
+      <c r="B64" s="7">
         <f>'Quick Sort'!W103</f>
         <v>2.1917070000000002E-3</v>
       </c>
-      <c r="C64" s="8">
+      <c r="C64" s="7">
         <f>'Quick Sort'!X103</f>
         <v>8.6616800000000017E-4</v>
       </c>
-      <c r="D64" s="8">
+      <c r="D64" s="7">
         <f>'Quick Sort'!Y103</f>
         <v>9.5374899999999994E-4</v>
       </c>
-      <c r="E64" s="8">
+      <c r="E64" s="7">
         <f>'Quick Sort'!Z103</f>
         <v>1.1025610000000002E-3</v>
       </c>
@@ -3780,19 +4339,19 @@
       <c r="A65">
         <v>100000</v>
       </c>
-      <c r="B65" s="8">
+      <c r="B65" s="7">
         <f>'Quick Sort'!AF103</f>
         <v>2.1917070000000002E-3</v>
       </c>
-      <c r="C65" s="8">
+      <c r="C65" s="7">
         <f>'Quick Sort'!AG103</f>
         <v>8.6616800000000017E-4</v>
       </c>
-      <c r="D65" s="8">
+      <c r="D65" s="7">
         <f>'Quick Sort'!AH103</f>
         <v>9.5374899999999994E-4</v>
       </c>
-      <c r="E65" s="8">
+      <c r="E65" s="7">
         <f>'Quick Sort'!AI103</f>
         <v>1.1025610000000002E-3</v>
       </c>
@@ -3801,171 +4360,403 @@
       <c r="A66">
         <v>1000000</v>
       </c>
-      <c r="B66" s="8">
+      <c r="B66" s="7">
         <f>'Quick Sort'!AO103</f>
         <v>0.29550432599999998</v>
       </c>
-      <c r="C66" s="8">
+      <c r="C66" s="7">
         <f>'Quick Sort'!AP103</f>
         <v>0.10307983000000001</v>
       </c>
-      <c r="D66" s="8">
+      <c r="D66" s="7">
         <f>'Quick Sort'!AQ103</f>
         <v>0.11240000399999998</v>
       </c>
-      <c r="E66" s="8">
+      <c r="E66" s="7">
         <f>'Quick Sort'!AR103</f>
         <v>0.11980461000000001</v>
       </c>
     </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="28"/>
+      <c r="C68" s="28"/>
+      <c r="D68" s="28"/>
+      <c r="E68" s="29"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1</v>
+      </c>
+      <c r="D69" t="s">
+        <v>2</v>
+      </c>
+      <c r="E69" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>10</v>
+      </c>
+      <c r="B70" s="6">
+        <v>2.8458014439847814E-7</v>
+      </c>
+      <c r="C70" s="6">
+        <v>1.5458971439904988E-7</v>
+      </c>
+      <c r="D70" s="6">
+        <v>2.8154515937532416E-7</v>
+      </c>
+      <c r="E70" s="6">
+        <v>2.0294797064242549E-7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>1000</v>
+      </c>
+      <c r="B71" s="6">
+        <v>1.3640288327471886E-5</v>
+      </c>
+      <c r="C71" s="6">
+        <v>7.1528390210185893E-6</v>
+      </c>
+      <c r="D71" s="6">
+        <v>8.174720827408154E-6</v>
+      </c>
+      <c r="E71" s="6">
+        <v>6.0913857871654103E-6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>10000</v>
+      </c>
+      <c r="B72" s="6">
+        <v>1.328877435083743E-4</v>
+      </c>
+      <c r="C72" s="6">
+        <v>6.5965145188940321E-5</v>
+      </c>
+      <c r="D72" s="6">
+        <v>7.9205618481203058E-5</v>
+      </c>
+      <c r="E72" s="6">
+        <v>4.5531201190152891E-5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>100000</v>
+      </c>
+      <c r="B73" s="6">
+        <v>1.328877435083743E-4</v>
+      </c>
+      <c r="C73" s="6">
+        <v>6.5965145188940321E-5</v>
+      </c>
+      <c r="D73" s="6">
+        <v>7.9205618481203058E-5</v>
+      </c>
+      <c r="E73" s="6">
+        <v>4.5531201190152891E-5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>1000000</v>
+      </c>
+      <c r="B74" s="6">
+        <v>6.5183923513669204E-3</v>
+      </c>
+      <c r="C74" s="6">
+        <v>3.2351134126061567E-3</v>
+      </c>
+      <c r="D74" s="6">
+        <v>7.5582902747361883E-4</v>
+      </c>
+      <c r="E74" s="6">
+        <v>8.5615079627341176E-4</v>
+      </c>
+    </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="28" t="s">
+      <c r="A80" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B80" s="29"/>
-      <c r="C80" s="29"/>
-      <c r="D80" s="29"/>
-      <c r="E80" s="30"/>
+      <c r="B80" s="28"/>
+      <c r="C80" s="28"/>
+      <c r="D80" s="28"/>
+      <c r="E80" s="29"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="25" t="s">
+      <c r="A81" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B81" s="12" t="s">
+      <c r="B81" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C81" s="12" t="s">
+      <c r="C81" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D81" s="12" t="s">
+      <c r="D81" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E81" s="26" t="s">
+      <c r="E81" s="22" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="16">
+      <c r="A82" s="12">
         <v>10</v>
       </c>
-      <c r="B82" s="17">
+      <c r="B82" s="13">
         <f>'Selection Sort'!E103</f>
         <v>7.8949999999999998E-6</v>
       </c>
-      <c r="C82" s="17">
+      <c r="C82" s="13">
         <f>'Selection Sort'!F103</f>
         <v>6.7950000000000002E-6</v>
       </c>
-      <c r="D82" s="17">
+      <c r="D82" s="13">
         <f>'Selection Sort'!G103</f>
         <v>6.6369999999999993E-6</v>
       </c>
-      <c r="E82" s="18">
+      <c r="E82" s="14">
         <f>'Selection Sort'!H103</f>
         <v>7.7449999999999978E-6</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="16">
+      <c r="A83" s="12">
         <v>1000</v>
       </c>
-      <c r="B83" s="17">
+      <c r="B83" s="13">
         <f>'Selection Sort'!N103</f>
         <v>1.6276840000000001E-3</v>
       </c>
-      <c r="C83" s="17">
+      <c r="C83" s="13">
         <f>'Selection Sort'!O103</f>
         <v>1.5517670000000001E-3</v>
       </c>
-      <c r="D83" s="17">
+      <c r="D83" s="13">
         <f>'Selection Sort'!P103</f>
         <v>1.5612359999999999E-3</v>
       </c>
-      <c r="E83" s="18">
+      <c r="E83" s="14">
         <f>'Selection Sort'!Q103</f>
         <v>1.5567300000000001E-3</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="16">
+      <c r="A84" s="12">
         <v>10000</v>
       </c>
-      <c r="B84" s="17">
+      <c r="B84" s="13">
         <f>'Selection Sort'!W103</f>
         <v>0.118933439</v>
       </c>
-      <c r="C84" s="17">
+      <c r="C84" s="13">
         <f>'Selection Sort'!X103</f>
         <v>0.11758300000000002</v>
       </c>
-      <c r="D84" s="17">
+      <c r="D84" s="13">
         <f>'Selection Sort'!Y103</f>
         <v>0.11229259899999999</v>
       </c>
-      <c r="E84" s="18">
+      <c r="E84" s="14">
         <f>'Selection Sort'!Z103</f>
         <v>0.11852893</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="16">
+      <c r="A85" s="12">
         <v>100000</v>
       </c>
-      <c r="B85" s="17">
+      <c r="B85" s="13">
         <f>'Selection Sort'!AF103</f>
         <v>10.44377538</v>
       </c>
-      <c r="C85" s="17">
+      <c r="C85" s="13">
         <f>'Selection Sort'!AG103</f>
         <v>11.227691418000001</v>
       </c>
-      <c r="D85" s="17">
+      <c r="D85" s="13">
         <f>'Selection Sort'!AH103</f>
         <v>9.9143543080000001</v>
       </c>
-      <c r="E85" s="18">
+      <c r="E85" s="14">
         <f>'Selection Sort'!AI103</f>
         <v>10.437320515</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="19">
+      <c r="A86" s="15">
         <v>1000000</v>
       </c>
-      <c r="B86" s="27" t="s">
+      <c r="B86" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C86" s="27" t="s">
+      <c r="C86" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D86" s="27" t="s">
+      <c r="D86" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E86" s="27" t="s">
+      <c r="E86" s="23" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B88" s="28"/>
+      <c r="C88" s="28"/>
+      <c r="D88" s="28"/>
+      <c r="E88" s="29"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E89" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="12">
+        <v>10</v>
+      </c>
+      <c r="B90" s="13">
+        <v>3.5306557893726059E-6</v>
+      </c>
+      <c r="C90" s="13">
+        <v>1.0920627317608684E-6</v>
+      </c>
+      <c r="D90" s="13">
+        <v>1.4552347167409387E-6</v>
+      </c>
+      <c r="E90" s="14">
+        <v>3.1300232354641476E-6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="12">
+        <v>1000</v>
+      </c>
+      <c r="B91" s="13">
+        <v>8.6882013016841361E-5</v>
+      </c>
+      <c r="C91" s="13">
+        <v>8.4458179304997807E-5</v>
+      </c>
+      <c r="D91" s="13">
+        <v>1.5258827980993013E-4</v>
+      </c>
+      <c r="E91" s="14">
+        <v>6.0320937115942217E-5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="12">
+        <v>10000</v>
+      </c>
+      <c r="B92" s="13">
+        <v>1.4603491357071455E-3</v>
+      </c>
+      <c r="C92" s="13">
+        <v>1.0981301700176669E-3</v>
+      </c>
+      <c r="D92" s="13">
+        <v>1.5095125169695934E-3</v>
+      </c>
+      <c r="E92" s="14">
+        <v>2.0989310197230288E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="12">
+        <v>100000</v>
+      </c>
+      <c r="B93" s="13">
+        <v>2.054442192565142E-2</v>
+      </c>
+      <c r="C93" s="13">
+        <v>0.38784382403153234</v>
+      </c>
+      <c r="D93" s="13">
+        <v>3.1631057610885652E-2</v>
+      </c>
+      <c r="E93" s="14">
+        <v>1.8334125083037878E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="15">
+        <v>1000000</v>
+      </c>
+      <c r="B94" s="23">
+        <v>6.2052619968747523E-2</v>
+      </c>
+      <c r="C94" s="23">
+        <v>2.5668923677006541E-4</v>
+      </c>
+      <c r="D94" s="23">
+        <v>2.5834897947630983E-4</v>
+      </c>
+      <c r="E94" s="23">
+        <v>2.2553333440507564E-4</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
+    <mergeCell ref="A88:E88"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A20:E20"/>
     <mergeCell ref="A80:E80"/>
     <mergeCell ref="A40:E40"/>
     <mergeCell ref="A60:E60"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A68:E68"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="5">
+  <tableParts count="10">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3977,71 +4768,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AR103"/>
+  <dimension ref="A1:AR104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView topLeftCell="AB73" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104:AR104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="13.625" customWidth="1"/>
+    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
     <col min="7" max="7" width="12.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.125" customWidth="1"/>
+    <col min="15" max="15" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="J1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="S1" s="3" t="s">
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="S1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AB1" s="3" t="s">
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AB1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AK1" s="3" t="s">
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AK1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3"/>
-      <c r="AR1" s="3"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -10409,7 +11202,7 @@
         <f t="shared" ref="F103:H103" si="13">AVERAGE(F3:F102)</f>
         <v>4.8539999999999996E-6</v>
       </c>
-      <c r="G103" s="5">
+      <c r="G103" s="4">
         <f t="shared" si="13"/>
         <v>4.4233545454545451E-5</v>
       </c>
@@ -10480,6 +11273,91 @@
       <c r="AR103">
         <f>AVERAGE(AR3:AR102)</f>
         <v>300.00177902000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>22</v>
+      </c>
+      <c r="E104" s="4">
+        <f>STDEV(A3:A102)</f>
+        <v>1.470327387442207E-6</v>
+      </c>
+      <c r="F104" s="4">
+        <f>STDEV(B3:B102)</f>
+        <v>1.4070113034658974E-6</v>
+      </c>
+      <c r="G104" s="4">
+        <f>STDEV(C3:C102)</f>
+        <v>5.5527839045751681E-6</v>
+      </c>
+      <c r="H104" s="4">
+        <f>STDEV(D3:D102)</f>
+        <v>1.4750394618929408E-6</v>
+      </c>
+      <c r="N104">
+        <f>STDEV(J3:J102)</f>
+        <v>2.5411264328230325E-3</v>
+      </c>
+      <c r="O104" s="4">
+        <f>STDEV(K3:K102)</f>
+        <v>1.8800075220137508E-5</v>
+      </c>
+      <c r="P104">
+        <f>STDEV(L3:L102)</f>
+        <v>1.6969268538996765E-3</v>
+      </c>
+      <c r="Q104">
+        <f>STDEV(M3:M102)</f>
+        <v>1.9606463604223395E-3</v>
+      </c>
+      <c r="W104">
+        <f>STDEV(S3:S102)</f>
+        <v>0.86529379593060129</v>
+      </c>
+      <c r="X104">
+        <f>STDEV(T3:T102)</f>
+        <v>1.0555058866570462E-4</v>
+      </c>
+      <c r="Y104">
+        <f>STDEV(U3:U102)</f>
+        <v>6.3345215171960865</v>
+      </c>
+      <c r="Z104">
+        <f>STDEV(V3:V102)</f>
+        <v>6.2093088639306222</v>
+      </c>
+      <c r="AF104">
+        <f>STDEV(AB3:AB102)</f>
+        <v>5.2580112643492445</v>
+      </c>
+      <c r="AG104">
+        <f>STDEV(AC3:AC102)</f>
+        <v>3.8448302900903133E-5</v>
+      </c>
+      <c r="AH104">
+        <f>STDEV(AD3:AD102)</f>
+        <v>11.508834093058141</v>
+      </c>
+      <c r="AI104">
+        <f>STDEV(AE3:AE102)</f>
+        <v>0.12167377308712887</v>
+      </c>
+      <c r="AO104">
+        <f>STDEV(AK3:AK26)</f>
+        <v>1.9492205014851657E-4</v>
+      </c>
+      <c r="AP104">
+        <f>STDEV(AL3:AL102)</f>
+        <v>9.4867000775141841E-4</v>
+      </c>
+      <c r="AQ104" s="4">
+        <f>STDEV(AM3:AM102)</f>
+        <v>1.8428451650695369E-4</v>
+      </c>
+      <c r="AR104" s="4">
+        <f>STDEV(AN3:AN102)</f>
+        <v>3.5724276574394267E-3</v>
       </c>
     </row>
   </sheetData>
@@ -10491,7 +11369,7 @@
     <mergeCell ref="AK1:AR1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -10502,68 +11380,72 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AR103"/>
+  <dimension ref="A1:AR104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AP103" sqref="AP103"/>
+    <sheetView topLeftCell="AH79" workbookViewId="0">
+      <selection activeCell="AM106" sqref="AM106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="8" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="23" max="26" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="41" max="44" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="J1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="S1" s="3" t="s">
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="S1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AB1" s="3" t="s">
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AB1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AK1" s="3" t="s">
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AK1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3"/>
-      <c r="AR1" s="3"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -17227,6 +18109,108 @@
       <c r="AR103">
         <f t="shared" si="170"/>
         <v>300.00124903833336</v>
+      </c>
+    </row>
+    <row r="104" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="E104" s="4">
+        <f>STDEV(A3:A102)</f>
+        <v>1.7118422942561176E-7</v>
+      </c>
+      <c r="F104" s="4">
+        <f>STDEV(B3:B102)</f>
+        <v>9.9478640923567117E-7</v>
+      </c>
+      <c r="G104" s="4">
+        <f>STDEV(C3:C102)</f>
+        <v>2.2879736083100335E-6</v>
+      </c>
+      <c r="H104" s="4">
+        <f>STDEV(D3:D102)</f>
+        <v>1.7401671811012304E-7</v>
+      </c>
+      <c r="I104" s="4"/>
+      <c r="J104" s="4"/>
+      <c r="K104" s="4"/>
+      <c r="L104" s="4"/>
+      <c r="M104" s="4"/>
+      <c r="N104" s="4">
+        <f>STDEV(J3:J102)</f>
+        <v>9.963815235540048E-4</v>
+      </c>
+      <c r="O104" s="4">
+        <f>STDEV(K3:K102)</f>
+        <v>1.5392411714342832E-5</v>
+      </c>
+      <c r="P104" s="4">
+        <f>STDEV(L3:L102)</f>
+        <v>5.8288469775689888E-3</v>
+      </c>
+      <c r="Q104" s="4">
+        <f>STDEV(M3:M102)</f>
+        <v>3.9522798981132747E-4</v>
+      </c>
+      <c r="R104" s="4"/>
+      <c r="S104" s="4"/>
+      <c r="T104" s="4"/>
+      <c r="U104" s="4"/>
+      <c r="V104" s="4"/>
+      <c r="W104" s="4">
+        <f>STDEV(S3:S102)</f>
+        <v>1.8254461088417107E-2</v>
+      </c>
+      <c r="X104" s="4">
+        <f>STDEV(T3:T102)</f>
+        <v>1.2761044786000205E-4</v>
+      </c>
+      <c r="Y104" s="4">
+        <f>STDEV(U3:U102)</f>
+        <v>0.47025357698834208</v>
+      </c>
+      <c r="Z104" s="4">
+        <f>STDEV(V3:V102)</f>
+        <v>7.7188260918710531E-3</v>
+      </c>
+      <c r="AA104" s="4"/>
+      <c r="AB104" s="4"/>
+      <c r="AC104" s="4"/>
+      <c r="AD104" s="4"/>
+      <c r="AE104" s="4"/>
+      <c r="AF104" s="4">
+        <f>STDEV(AB3:AB102)</f>
+        <v>5.530829561711295</v>
+      </c>
+      <c r="AG104" s="4">
+        <f>STDEV(AC3:AC102)</f>
+        <v>7.1561162651259333E-7</v>
+      </c>
+      <c r="AH104" s="4">
+        <f>STDEV(AD3:AD102)</f>
+        <v>2.3010540984013677</v>
+      </c>
+      <c r="AI104" s="4">
+        <f>STDEV(AE3:AE102)</f>
+        <v>0.20056533128894721</v>
+      </c>
+      <c r="AJ104" s="4"/>
+      <c r="AK104" s="4"/>
+      <c r="AL104" s="4"/>
+      <c r="AM104" s="4"/>
+      <c r="AN104" s="4"/>
+      <c r="AO104" s="4">
+        <f>STDEV(AK3:AK26)</f>
+        <v>2.1708322383141515E-4</v>
+      </c>
+      <c r="AP104" s="4">
+        <f>STDEV(AL3:AL102)</f>
+        <v>1.6913334252350045E-3</v>
+      </c>
+      <c r="AQ104" s="4">
+        <f>STDEV(AM3:AM26)</f>
+        <v>2.296116753316763E-4</v>
+      </c>
+      <c r="AR104" s="4">
+        <f>STDEV(AN3:AN26)</f>
+        <v>2.5071576402001185E-4</v>
       </c>
     </row>
   </sheetData>
@@ -17249,10 +18233,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AR103"/>
+  <dimension ref="A1:AR104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AR103"/>
+    <sheetView topLeftCell="AA97" workbookViewId="0">
+      <selection activeCell="AO104" sqref="AO104:AR104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -17261,56 +18245,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="J1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="S1" s="3" t="s">
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="S1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AB1" s="3" t="s">
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AB1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AK1" s="3" t="s">
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AK1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3"/>
-      <c r="AR1" s="3"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -24514,6 +25498,88 @@
       <c r="AR103">
         <f t="shared" ref="AR103" si="213">AVERAGE(AR3:AR102)</f>
         <v>0.42739784199999997</v>
+      </c>
+    </row>
+    <row r="104" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="E104">
+        <f>STDEV(A3:A102)</f>
+        <v>1.6695523503337799E-6</v>
+      </c>
+      <c r="F104">
+        <f>STDEV(B3:B102)</f>
+        <v>8.0524229367014222E-7</v>
+      </c>
+      <c r="G104">
+        <f>STDEV(C3:C102)</f>
+        <v>1.1447799841546905E-6</v>
+      </c>
+      <c r="H104">
+        <f>STDEV(D3:D102)</f>
+        <v>1.744792830166957E-6</v>
+      </c>
+      <c r="N104">
+        <f>STDEV(J3:J102)</f>
+        <v>5.6920054835042489E-5</v>
+      </c>
+      <c r="O104">
+        <f>STDEV(K3:K102)</f>
+        <v>5.4301631009602555E-5</v>
+      </c>
+      <c r="P104">
+        <f>STDEV(L3:L102)</f>
+        <v>5.0802322821308116E-5</v>
+      </c>
+      <c r="Q104">
+        <f>STDEV(M3:M102)</f>
+        <v>4.9964036116495887E-5</v>
+      </c>
+      <c r="W104">
+        <f>STDEV(S3:S102)</f>
+        <v>1.7525698245430881E-4</v>
+      </c>
+      <c r="X104">
+        <f>STDEV(T3:T102)</f>
+        <v>2.5038249005120627E-4</v>
+      </c>
+      <c r="Y104">
+        <f>STDEV(U3:U102)</f>
+        <v>1.3628676310254673E-4</v>
+      </c>
+      <c r="Z104">
+        <f>STDEV(V3:V102)</f>
+        <v>2.1338285016951253E-4</v>
+      </c>
+      <c r="AF104">
+        <f>STDEV(AB3:AB102)</f>
+        <v>1.4084242268979647E-3</v>
+      </c>
+      <c r="AG104">
+        <f>STDEV(AC3:AC102)</f>
+        <v>3.3661465676120559E-4</v>
+      </c>
+      <c r="AH104">
+        <f>STDEV(AD3:AD102)</f>
+        <v>2.3527113952830973E-4</v>
+      </c>
+      <c r="AI104">
+        <f>STDEV(AE3:AE102)</f>
+        <v>2.6734594316969322E-4</v>
+      </c>
+      <c r="AO104">
+        <f>STDEV(AK3:AK26)</f>
+        <v>4.6078095028255737E-3</v>
+      </c>
+      <c r="AP104">
+        <f>STDEV(AL3:AL102)</f>
+        <v>1.6366821042893495E-3</v>
+      </c>
+      <c r="AQ104">
+        <f>STDEV(AM3:AM102)</f>
+        <v>1.7182035205423236E-3</v>
+      </c>
+      <c r="AR104">
+        <f>STDEV(AN3:AN102)</f>
+        <v>1.9109431687990618E-3</v>
       </c>
     </row>
   </sheetData>
@@ -24536,10 +25602,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AR103"/>
+  <dimension ref="A1:AR104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AR103"/>
+    <sheetView topLeftCell="AB88" workbookViewId="0">
+      <selection activeCell="AO104" sqref="AO104:AR104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -24548,56 +25614,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="J1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="S1" s="3" t="s">
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="S1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AB1" s="3" t="s">
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AB1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AK1" s="3" t="s">
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AK1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3"/>
-      <c r="AR1" s="3"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -31801,6 +32867,88 @@
       <c r="AR103">
         <f t="shared" si="54"/>
         <v>0.11980461000000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="E104">
+        <f>STDEV(A3:A102)</f>
+        <v>2.8458014439847814E-7</v>
+      </c>
+      <c r="F104">
+        <f>STDEV(B3:B102)</f>
+        <v>1.5458971439904988E-7</v>
+      </c>
+      <c r="G104">
+        <f>STDEV(C3:C102)</f>
+        <v>2.8154515937532416E-7</v>
+      </c>
+      <c r="H104">
+        <f>STDEV(D3:D102)</f>
+        <v>2.0294797064242549E-7</v>
+      </c>
+      <c r="N104">
+        <f>STDEV(J3:J102)</f>
+        <v>1.3640288327471886E-5</v>
+      </c>
+      <c r="O104">
+        <f>STDEV(K3:K102)</f>
+        <v>7.1528390210185893E-6</v>
+      </c>
+      <c r="P104">
+        <f>STDEV(L3:L102)</f>
+        <v>8.174720827408154E-6</v>
+      </c>
+      <c r="Q104">
+        <f>STDEV(M3:M102)</f>
+        <v>6.0913857871654103E-6</v>
+      </c>
+      <c r="W104">
+        <f>STDEV(S3:S102)</f>
+        <v>1.328877435083743E-4</v>
+      </c>
+      <c r="X104">
+        <f>STDEV(T3:T102)</f>
+        <v>6.5965145188940321E-5</v>
+      </c>
+      <c r="Y104">
+        <f>STDEV(U3:U102)</f>
+        <v>7.9205618481203058E-5</v>
+      </c>
+      <c r="Z104">
+        <f>STDEV(V3:V102)</f>
+        <v>4.5531201190152891E-5</v>
+      </c>
+      <c r="AF104">
+        <f>STDEV(AB3:AB102)</f>
+        <v>1.328877435083743E-4</v>
+      </c>
+      <c r="AG104">
+        <f>STDEV(AC3:AC102)</f>
+        <v>6.5965145188940321E-5</v>
+      </c>
+      <c r="AH104">
+        <f>STDEV(AD3:AD102)</f>
+        <v>7.9205618481203058E-5</v>
+      </c>
+      <c r="AI104">
+        <f>STDEV(AE3:AE102)</f>
+        <v>4.5531201190152891E-5</v>
+      </c>
+      <c r="AO104">
+        <f>STDEV(AK3:AK26)</f>
+        <v>6.5183923513669204E-3</v>
+      </c>
+      <c r="AP104">
+        <f>STDEV(AL3:AL102)</f>
+        <v>3.2351134126061567E-3</v>
+      </c>
+      <c r="AQ104">
+        <f>STDEV(AM3:AM102)</f>
+        <v>7.5582902747361883E-4</v>
+      </c>
+      <c r="AR104">
+        <f>STDEV(AN3:AN102)</f>
+        <v>8.5615079627341176E-4</v>
       </c>
     </row>
   </sheetData>
@@ -31823,10 +32971,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AR103"/>
+  <dimension ref="A1:AR104"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AF17" sqref="AF17"/>
+    <sheetView topLeftCell="AA66" workbookViewId="0">
+      <selection activeCell="AO104" sqref="AO104:AR104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -31835,56 +32983,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="J1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="S1" s="3" t="s">
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="S1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AB1" s="3" t="s">
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AB1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
-      <c r="AH1" s="3"/>
-      <c r="AI1" s="3"/>
-      <c r="AK1" s="3" t="s">
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AK1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="3"/>
-      <c r="AQ1" s="3"/>
-      <c r="AR1" s="3"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -38064,6 +39212,88 @@
       <c r="AR103">
         <f t="shared" si="49"/>
         <v>300.00120764833332</v>
+      </c>
+    </row>
+    <row r="104" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="E104">
+        <f>STDEV(A3:A102)</f>
+        <v>3.5306557893726059E-6</v>
+      </c>
+      <c r="F104">
+        <f>STDEV(B3:B102)</f>
+        <v>1.0920627317608684E-6</v>
+      </c>
+      <c r="G104">
+        <f>STDEV(C3:C102)</f>
+        <v>1.4552347167409387E-6</v>
+      </c>
+      <c r="H104">
+        <f>STDEV(D3:D102)</f>
+        <v>3.1300232354641476E-6</v>
+      </c>
+      <c r="N104">
+        <f>STDEV(J3:J102)</f>
+        <v>8.6882013016841361E-5</v>
+      </c>
+      <c r="O104">
+        <f>STDEV(K3:K102)</f>
+        <v>8.4458179304997807E-5</v>
+      </c>
+      <c r="P104">
+        <f>STDEV(L3:L102)</f>
+        <v>1.5258827980993013E-4</v>
+      </c>
+      <c r="Q104">
+        <f>STDEV(M3:M102)</f>
+        <v>6.0320937115942217E-5</v>
+      </c>
+      <c r="W104">
+        <f>STDEV(S3:S102)</f>
+        <v>1.4603491357071455E-3</v>
+      </c>
+      <c r="X104">
+        <f>STDEV(T3:T102)</f>
+        <v>1.0981301700176669E-3</v>
+      </c>
+      <c r="Y104">
+        <f>STDEV(U3:U102)</f>
+        <v>1.5095125169695934E-3</v>
+      </c>
+      <c r="Z104">
+        <f>STDEV(V3:V102)</f>
+        <v>2.0989310197230288E-3</v>
+      </c>
+      <c r="AF104">
+        <f>STDEV(AB3:AB102)</f>
+        <v>2.054442192565142E-2</v>
+      </c>
+      <c r="AG104">
+        <f>STDEV(AC3:AC102)</f>
+        <v>0.38784382403153234</v>
+      </c>
+      <c r="AH104">
+        <f>STDEV(AD3:AD102)</f>
+        <v>3.1631057610885652E-2</v>
+      </c>
+      <c r="AI104">
+        <f>STDEV(AE3:AE102)</f>
+        <v>1.8334125083037878E-2</v>
+      </c>
+      <c r="AO104">
+        <f>STDEV(AK3:AK26)</f>
+        <v>6.2052619968747523E-2</v>
+      </c>
+      <c r="AP104">
+        <f>STDEV(AL3:AL102)</f>
+        <v>2.5668923677006541E-4</v>
+      </c>
+      <c r="AQ104">
+        <f>STDEV(AM3:AM102)</f>
+        <v>2.5834897947630983E-4</v>
+      </c>
+      <c r="AR104">
+        <f>STDEV(AN3:AN102)</f>
+        <v>2.2553333440507564E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>